<commit_message>
GameManager done, PrefabManager almost complete, started Player class and animations with Directions and States
</commit_message>
<xml_diff>
--- a/C61/Sprint 1/Planification.xlsx
+++ b/C61/Sprint 1/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\ProjetFinalC61\C61\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D183053-2600-4FE2-8F53-2DB5BC14318E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4311D5B-539E-4C97-8630-9657173C9578}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11BE00C6-C346-4921-8AF1-FC1656D8A7FD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>Tâche</t>
   </si>
@@ -157,23 +157,19 @@
   </si>
   <si>
     <t>Temps</t>
+  </si>
+  <si>
+    <t>Oui</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,6 +220,29 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF002060"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -331,45 +350,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,7 +720,7 @@
   <dimension ref="B1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,15 +737,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="45.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="3" spans="2:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -741,16 +769,16 @@
       <c r="H3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="N3" s="10" t="s">
         <v>37</v>
       </c>
     </row>
@@ -771,13 +799,13 @@
       <c r="G4" s="7">
         <v>120</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="M4" s="14" t="s">
+      <c r="H4" s="15"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="17"/>
+      <c r="M4" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="12">
         <v>1875</v>
       </c>
     </row>
@@ -800,15 +828,19 @@
       <c r="G5" s="7">
         <v>90</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="M5" s="14" t="s">
+      <c r="H5" s="15">
+        <v>60</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="17"/>
+      <c r="M5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="12">
         <f>SUM(H4:H21)</f>
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -830,9 +862,9 @@
       <c r="G6" s="7">
         <v>180</v>
       </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
@@ -851,9 +883,9 @@
       <c r="G7" s="7">
         <v>90</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17"/>
     </row>
     <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
@@ -874,9 +906,9 @@
       <c r="G8" s="7">
         <v>30</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17"/>
     </row>
     <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
@@ -897,9 +929,9 @@
       <c r="G9" s="7">
         <v>120</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
@@ -918,9 +950,9 @@
       <c r="G10" s="7">
         <v>45</v>
       </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="17"/>
     </row>
     <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
@@ -941,9 +973,10 @@
       <c r="G11" s="7">
         <v>90</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="17"/>
+      <c r="M11" s="18"/>
     </row>
     <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
@@ -964,9 +997,9 @@
       <c r="G12" s="7">
         <v>30</v>
       </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="17"/>
     </row>
     <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
@@ -987,9 +1020,9 @@
       <c r="G13" s="7">
         <v>60</v>
       </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="17"/>
     </row>
     <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
@@ -1008,9 +1041,9 @@
       <c r="G14" s="7">
         <v>240</v>
       </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
@@ -1031,9 +1064,9 @@
       <c r="G15" s="7">
         <v>60</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="17"/>
     </row>
     <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
@@ -1054,9 +1087,9 @@
       <c r="G16" s="7">
         <v>120</v>
       </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="17"/>
     </row>
     <row r="17" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
@@ -1077,9 +1110,9 @@
       <c r="G17" s="7">
         <v>120</v>
       </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="17"/>
     </row>
     <row r="18" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
@@ -1098,9 +1131,9 @@
       <c r="G18" s="7">
         <v>90</v>
       </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="17"/>
     </row>
     <row r="19" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
@@ -1119,9 +1152,9 @@
       <c r="G19" s="7">
         <v>90</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="17"/>
     </row>
     <row r="20" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
@@ -1140,9 +1173,9 @@
       <c r="G20" s="7">
         <v>60</v>
       </c>
-      <c r="H20" s="7"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="17"/>
     </row>
     <row r="21" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
@@ -1163,9 +1196,9 @@
       <c r="G21" s="7">
         <v>240</v>
       </c>
-      <c r="H21" s="7"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="17"/>
     </row>
     <row r="22" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modified MovementController for move start/stop detection
</commit_message>
<xml_diff>
--- a/C61/Sprint 1/Planification.xlsx
+++ b/C61/Sprint 1/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\ProjetFinalC61\C61\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4311D5B-539E-4C97-8630-9657173C9578}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C4CB1F-C84A-4EE5-8F78-82488ED9B307}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11BE00C6-C346-4921-8AF1-FC1656D8A7FD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
   <si>
     <t>Tâche</t>
   </si>
@@ -160,6 +160,18 @@
   </si>
   <si>
     <t>Oui</t>
+  </si>
+  <si>
+    <t>Ajouts</t>
+  </si>
+  <si>
+    <t>FacingController (détection 8-direction)</t>
+  </si>
+  <si>
+    <t>Difficile</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -248,7 +260,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,6 +294,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -350,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -382,22 +400,26 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2D228D-ED81-450E-98C6-898DFE30E920}">
-  <dimension ref="B1:N25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,15 +759,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="45.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="3" spans="2:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -799,9 +821,13 @@
       <c r="G4" s="7">
         <v>120</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="17"/>
+      <c r="H4" s="13">
+        <v>80</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="15"/>
       <c r="M4" s="11" t="s">
         <v>38</v>
       </c>
@@ -828,19 +854,19 @@
       <c r="G5" s="7">
         <v>90</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="13">
         <v>60</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="17"/>
+      <c r="J5" s="15"/>
       <c r="M5" s="11" t="s">
         <v>39</v>
       </c>
       <c r="N5" s="12">
         <f>SUM(H4:H21)</f>
-        <v>60</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -862,9 +888,9 @@
       <c r="G6" s="7">
         <v>180</v>
       </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="17"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
@@ -883,9 +909,9 @@
       <c r="G7" s="7">
         <v>90</v>
       </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="17"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="15"/>
     </row>
     <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
@@ -906,9 +932,9 @@
       <c r="G8" s="7">
         <v>30</v>
       </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="17"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="15"/>
     </row>
     <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
@@ -929,9 +955,9 @@
       <c r="G9" s="7">
         <v>120</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="17"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="15"/>
     </row>
     <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
@@ -950,9 +976,9 @@
       <c r="G10" s="7">
         <v>45</v>
       </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="17"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="15"/>
     </row>
     <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
@@ -973,10 +999,10 @@
       <c r="G11" s="7">
         <v>90</v>
       </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="17"/>
-      <c r="M11" s="18"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="15"/>
+      <c r="M11" s="16"/>
     </row>
     <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
@@ -997,9 +1023,9 @@
       <c r="G12" s="7">
         <v>30</v>
       </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="17"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
     </row>
     <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
@@ -1020,9 +1046,9 @@
       <c r="G13" s="7">
         <v>60</v>
       </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="17"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="15"/>
     </row>
     <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
@@ -1041,9 +1067,9 @@
       <c r="G14" s="7">
         <v>240</v>
       </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="17"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="15"/>
     </row>
     <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
@@ -1064,9 +1090,9 @@
       <c r="G15" s="7">
         <v>60</v>
       </c>
-      <c r="H15" s="15"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="17"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="15"/>
     </row>
     <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
@@ -1087,11 +1113,11 @@
       <c r="G16" s="7">
         <v>120</v>
       </c>
-      <c r="H16" s="15"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17"/>
-    </row>
-    <row r="17" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="13"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
         <v>14</v>
       </c>
@@ -1110,11 +1136,11 @@
       <c r="G17" s="7">
         <v>120</v>
       </c>
-      <c r="H17" s="15"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="17"/>
-    </row>
-    <row r="18" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="13"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <v>15</v>
       </c>
@@ -1131,11 +1157,11 @@
       <c r="G18" s="7">
         <v>90</v>
       </c>
-      <c r="H18" s="15"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="17"/>
-    </row>
-    <row r="19" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="13"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
         <v>16</v>
       </c>
@@ -1152,11 +1178,11 @@
       <c r="G19" s="7">
         <v>90</v>
       </c>
-      <c r="H19" s="15"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="17"/>
-    </row>
-    <row r="20" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="13"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="15"/>
+    </row>
+    <row r="20" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>17</v>
       </c>
@@ -1173,11 +1199,11 @@
       <c r="G20" s="7">
         <v>60</v>
       </c>
-      <c r="H20" s="15"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="17"/>
-    </row>
-    <row r="21" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="13"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="15"/>
+    </row>
+    <row r="21" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
         <v>18</v>
       </c>
@@ -1196,14 +1222,32 @@
       <c r="G21" s="7">
         <v>240</v>
       </c>
-      <c r="H21" s="15"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="17"/>
-    </row>
-    <row r="22" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="15"/>
+    </row>
+    <row r="22" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+    </row>
+    <row r="23" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:H1"/>

</xml_diff>

<commit_message>
Skeleton and SimpleEnemy classes done, player attack and sword collision started
Skeleton uses SimpleEnemy, which takes care of all damage/health/OnHit/OnDeath behaviors for basic, minion type enemies to avoid repeating same code. Spawner summons new Skeletons on a timer. Player can now attack and kill enemies. Sword attack and collision detection still finicky
</commit_message>
<xml_diff>
--- a/C61/Sprint 1/Planification.xlsx
+++ b/C61/Sprint 1/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\ProjetFinalC61\C61\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C4CB1F-C84A-4EE5-8F78-82488ED9B307}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73622F81-07F4-4963-9053-43904E9FB762}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11BE00C6-C346-4921-8AF1-FC1656D8A7FD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
   <si>
     <t>Tâche</t>
   </si>
@@ -171,14 +171,41 @@
     <t>Difficile</t>
   </si>
   <si>
-    <t>-</t>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>Non complété</t>
+  </si>
+  <si>
+    <t>Prefab Manager (refactor platformer)</t>
+  </si>
+  <si>
+    <t>Movement Controller (refactor platformer)</t>
+  </si>
+  <si>
+    <t>Create Hero prefab</t>
+  </si>
+  <si>
+    <t>Create first platformer level</t>
+  </si>
+  <si>
+    <t>Commentaires</t>
+  </si>
+  <si>
+    <t>Problème au niveau du facing gauche/droite</t>
+  </si>
+  <si>
+    <t>Problème au niveau de la caméra qui suit la position du joueur et l'emplacement de la map</t>
+  </si>
+  <si>
+    <t>Doit être modifié car plus d'animation 8 direction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,6 +286,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FF002060"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -304,7 +355,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -364,11 +415,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -416,10 +476,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,26 +820,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2D228D-ED81-450E-98C6-898DFE30E920}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="40.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42.85546875" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
     <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="89.140625" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
     <col min="14" max="14" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="45.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="17" t="s">
         <v>33</v>
       </c>
@@ -769,7 +852,7 @@
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
     </row>
-    <row r="3" spans="2:14" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -797,14 +880,11 @@
       <c r="J3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>1</v>
       </c>
@@ -828,188 +908,199 @@
         <v>41</v>
       </c>
       <c r="J4" s="15"/>
-      <c r="M4" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" s="12">
-        <v>1875</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="22">
         <v>1</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="E5" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="23">
         <v>90</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="24">
         <v>60</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="26"/>
+    </row>
+    <row r="6" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="7">
+        <v>90</v>
+      </c>
+      <c r="H6" s="13">
+        <v>60</v>
+      </c>
+      <c r="I6" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="15"/>
-      <c r="M5" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="N5" s="12">
-        <f>SUM(H4:H21)</f>
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4">
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="E7" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G7" s="23">
         <v>180</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="15"/>
-    </row>
-    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="4">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="7" t="s">
+      <c r="H7" s="24">
+        <v>210</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="26"/>
+      <c r="L7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="7">
-        <v>90</v>
-      </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15"/>
-    </row>
-    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
-        <v>5</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="6">
-        <v>2</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>10</v>
-      </c>
       <c r="G8" s="7">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="H8" s="13"/>
       <c r="I8" s="14"/>
       <c r="J8" s="15"/>
-    </row>
-    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
-        <v>6</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="7">
-        <v>120</v>
-      </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="14"/>
+        <v>4</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="23">
+        <v>90</v>
+      </c>
+      <c r="H9" s="24">
+        <v>90</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>46</v>
+      </c>
       <c r="J9" s="15"/>
     </row>
-    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
-        <v>7</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G10" s="7">
-        <v>45</v>
+        <v>300</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="14"/>
       <c r="J10" s="15"/>
-    </row>
-    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
-        <v>8</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="7">
-        <v>90</v>
-      </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="14"/>
+        <v>5</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="22">
+        <v>2</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="23">
+        <v>30</v>
+      </c>
+      <c r="H11" s="24">
+        <v>30</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>41</v>
+      </c>
       <c r="J11" s="15"/>
-      <c r="M11" s="16"/>
-    </row>
-    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
-        <v>9</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="D12" s="6">
         <v>2</v>
@@ -1023,19 +1114,21 @@
       <c r="G12" s="7">
         <v>30</v>
       </c>
-      <c r="H12" s="13"/>
+      <c r="H12" s="13">
+        <v>30</v>
+      </c>
       <c r="I12" s="14"/>
       <c r="J12" s="15"/>
     </row>
-    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>7</v>
@@ -1044,210 +1137,332 @@
         <v>10</v>
       </c>
       <c r="G13" s="7">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="14"/>
       <c r="J13" s="15"/>
     </row>
-    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G14" s="7">
-        <v>240</v>
+        <v>45</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="14"/>
       <c r="J14" s="15"/>
     </row>
-    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G15" s="7">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="14"/>
       <c r="J15" s="15"/>
-    </row>
-    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M15" s="16"/>
+    </row>
+    <row r="16" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
-        <v>13</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="7">
-        <v>120</v>
-      </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="14"/>
+        <v>9</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="22">
+        <v>2</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="23">
+        <v>30</v>
+      </c>
+      <c r="H16" s="24"/>
+      <c r="I16" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="J16" s="15"/>
     </row>
-    <row r="17" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
-        <v>14</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="6">
-        <v>1</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="7">
-        <v>120</v>
-      </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="14"/>
+        <v>10</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="23">
+        <v>60</v>
+      </c>
+      <c r="H17" s="24"/>
+      <c r="I17" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="J17" s="15"/>
     </row>
-    <row r="18" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G18" s="7">
-        <v>90</v>
+        <v>240</v>
       </c>
       <c r="H18" s="13"/>
       <c r="I18" s="14"/>
       <c r="J18" s="15"/>
     </row>
-    <row r="19" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
-        <v>16</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="E19" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G19" s="7">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="H19" s="13"/>
       <c r="I19" s="14"/>
       <c r="J19" s="15"/>
     </row>
-    <row r="20" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="E20" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G20" s="7">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="H20" s="13"/>
       <c r="I20" s="14"/>
       <c r="J20" s="15"/>
     </row>
-    <row r="21" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D21" s="6">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="G21" s="7">
-        <v>240</v>
+        <v>120</v>
       </c>
       <c r="H21" s="13"/>
       <c r="I21" s="14"/>
       <c r="J21" s="15"/>
     </row>
-    <row r="22" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>15</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="7">
+        <v>90</v>
+      </c>
+      <c r="H22" s="13"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="15"/>
+    </row>
+    <row r="23" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <v>16</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="7">
+        <v>90</v>
+      </c>
+      <c r="H23" s="13"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="15"/>
+    </row>
+    <row r="24" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>17</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="7">
+        <v>60</v>
+      </c>
+      <c r="H24" s="13"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="15"/>
+    </row>
+    <row r="25" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>18</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="6">
+        <v>8</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="7">
+        <v>240</v>
+      </c>
+      <c r="H25" s="13"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="15"/>
+    </row>
+    <row r="26" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C26" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20" t="s">
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-    </row>
-    <row r="23" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="G26" s="20">
+        <v>120</v>
+      </c>
+      <c r="H26" s="20">
+        <v>300</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26" s="20"/>
+    </row>
+    <row r="27" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M28" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="N28" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M29" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N29" s="12">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M30" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="N30" s="12">
+        <f>SUM(H4:H26)</f>
+        <v>860</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:H1"/>

</xml_diff>

<commit_message>
MainMenu animation with StartGame option + fade in/fade out transition to next level
</commit_message>
<xml_diff>
--- a/C61/Sprint 1/Planification.xlsx
+++ b/C61/Sprint 1/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\ProjetFinalC61\C61\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73622F81-07F4-4963-9053-43904E9FB762}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7D20C7-7D89-4BB9-8DE8-D874A77D03E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11BE00C6-C346-4921-8AF1-FC1656D8A7FD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="71">
   <si>
     <t>Tâche</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Main Menu</t>
   </si>
   <si>
-    <t>Scene Manager</t>
-  </si>
-  <si>
     <t>Quest Manager</t>
   </si>
   <si>
@@ -195,17 +192,68 @@
     <t>Problème au niveau du facing gauche/droite</t>
   </si>
   <si>
-    <t>Problème au niveau de la caméra qui suit la position du joueur et l'emplacement de la map</t>
-  </si>
-  <si>
     <t>Doit être modifié car plus d'animation 8 direction</t>
+  </si>
+  <si>
+    <t>% complété</t>
+  </si>
+  <si>
+    <t>90-95%</t>
+  </si>
+  <si>
+    <t>Quelques ajouts seront nécessaires pour les prochains levels</t>
+  </si>
+  <si>
+    <t>Quelques ajouts à faire lorsque des nouveaux personnages/objets seront créés</t>
+  </si>
+  <si>
+    <t>Long car a dû être refait, plusieurs bugs d'animation, beaucoup de lecture de doc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas de menu ou autre level pour le moment </t>
+  </si>
+  <si>
+    <t>Finir un level complet et débuggé + main menu en priorité</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>100%</t>
+  </si>
+  <si>
+    <t>75%</t>
+  </si>
+  <si>
+    <t>Quelques animations pourraient s'ajouter</t>
+  </si>
+  <si>
+    <t>70%</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>40%</t>
+  </si>
+  <si>
+    <t>Level Manager</t>
+  </si>
+  <si>
+    <t>Pas de changement de level pour le moment</t>
+  </si>
+  <si>
+    <t>Problème avec map et caméra qui suit le joueur, difficulté à détecter collisions correctement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plus long dû au changement de projet et gestion des colliders frame par frame </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,8 +358,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF660033"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -354,8 +409,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -424,11 +485,82 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -466,16 +598,7 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -495,11 +618,37 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -509,6 +658,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF660033"/>
       <color rgb="FFFF9999"/>
     </mruColors>
   </colors>
@@ -822,36 +972,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2D228D-ED81-450E-98C6-898DFE30E920}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="42.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="12" max="12" width="89.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="30"/>
+    <col min="12" max="12" width="100.140625" customWidth="1"/>
     <col min="13" max="13" width="15.28515625" customWidth="1"/>
     <col min="14" max="14" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-    </row>
+      <c r="B1" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+    </row>
+    <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -872,19 +1025,22 @@
         <v>5</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>1</v>
       </c>
@@ -905,43 +1061,53 @@
         <v>80</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="15"/>
-    </row>
-    <row r="5" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="J4" s="26"/>
+      <c r="K4" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="19">
         <v>1</v>
       </c>
-      <c r="E5" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="23" t="s">
+      <c r="E5" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="20">
         <v>90</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="21">
         <v>60</v>
       </c>
-      <c r="I5" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" s="26"/>
-    </row>
-    <row r="6" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="27"/>
+      <c r="K5" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="L5" s="25"/>
+    </row>
+    <row r="6" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>2.1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
@@ -959,46 +1125,55 @@
         <v>60</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="15"/>
-    </row>
-    <row r="7" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="J6" s="26"/>
+      <c r="K6" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="23" t="s">
+      <c r="E7" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="20">
         <v>180</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="21">
         <v>210</v>
       </c>
-      <c r="I7" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="26"/>
-      <c r="L7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="27"/>
+      <c r="K7" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>3.1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>12</v>
@@ -1012,44 +1187,53 @@
       <c r="G8" s="7">
         <v>180</v>
       </c>
-      <c r="H8" s="13"/>
+      <c r="H8" s="13">
+        <v>220</v>
+      </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="15"/>
-      <c r="L8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="26"/>
+      <c r="K8" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>4</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="23" t="s">
+      <c r="D9" s="19"/>
+      <c r="E9" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="20">
         <v>90</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="21">
         <v>90</v>
       </c>
-      <c r="I9" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" s="15"/>
-    </row>
-    <row r="10" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="26"/>
+      <c r="K9" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9" s="25"/>
+    </row>
+    <row r="10" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>4.0999999999999996</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7" t="s">
@@ -1061,46 +1245,55 @@
       <c r="G10" s="7">
         <v>300</v>
       </c>
-      <c r="H10" s="13"/>
+      <c r="H10" s="13">
+        <v>500</v>
+      </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="15"/>
-      <c r="L10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="26"/>
+      <c r="K10" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="L10" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <v>5</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="19">
         <v>2</v>
       </c>
-      <c r="E11" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="23" t="s">
+      <c r="E11" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="20">
         <v>30</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="21">
         <v>30</v>
       </c>
-      <c r="I11" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="J11" s="15"/>
-    </row>
-    <row r="12" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="26"/>
+      <c r="K11" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="L11" s="25"/>
+    </row>
+    <row r="12" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>5.0999999999999996</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="6">
         <v>2</v>
@@ -1118,9 +1311,15 @@
         <v>30</v>
       </c>
       <c r="I12" s="14"/>
-      <c r="J12" s="15"/>
-    </row>
-    <row r="13" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="26"/>
+      <c r="K12" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12" s="25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>6</v>
       </c>
@@ -1139,11 +1338,19 @@
       <c r="G13" s="7">
         <v>120</v>
       </c>
-      <c r="H13" s="13"/>
+      <c r="H13" s="13">
+        <v>300</v>
+      </c>
       <c r="I13" s="14"/>
-      <c r="J13" s="15"/>
-    </row>
-    <row r="14" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="26"/>
+      <c r="K13" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="L13" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>7</v>
       </c>
@@ -1160,11 +1367,19 @@
       <c r="G14" s="7">
         <v>45</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="15"/>
-    </row>
-    <row r="15" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="13">
+        <v>30</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="26"/>
+      <c r="K14" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="L14" s="25"/>
+    </row>
+    <row r="15" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>8</v>
       </c>
@@ -1184,61 +1399,79 @@
         <v>90</v>
       </c>
       <c r="H15" s="13"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="15"/>
-      <c r="M15" s="16"/>
-    </row>
-    <row r="16" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="34">
+        <v>3</v>
+      </c>
+      <c r="K15" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="L15" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="M15" s="15"/>
+    </row>
+    <row r="16" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <v>9</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="19">
         <v>2</v>
       </c>
-      <c r="E16" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="23" t="s">
+      <c r="E16" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="20">
         <v>30</v>
       </c>
-      <c r="H16" s="24"/>
-      <c r="I16" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="J16" s="15"/>
-    </row>
-    <row r="17" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="21"/>
+      <c r="I16" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="J16" s="26"/>
+      <c r="K16" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" s="25"/>
+    </row>
+    <row r="17" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
         <v>10</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="23" t="s">
+      <c r="E17" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="20">
         <v>60</v>
       </c>
-      <c r="H17" s="24"/>
-      <c r="I17" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="21"/>
+      <c r="I17" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="J17" s="26"/>
+      <c r="K17" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="L17" s="25"/>
+    </row>
+    <row r="18" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <v>11</v>
       </c>
@@ -1255,11 +1488,19 @@
       <c r="G18" s="7">
         <v>240</v>
       </c>
-      <c r="H18" s="13"/>
+      <c r="H18" s="13">
+        <v>500</v>
+      </c>
       <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
-    </row>
-    <row r="19" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J18" s="26"/>
+      <c r="K18" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="L18" s="25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
         <v>12</v>
       </c>
@@ -1280,14 +1521,16 @@
       </c>
       <c r="H19" s="13"/>
       <c r="I19" s="14"/>
-      <c r="J19" s="15"/>
-    </row>
-    <row r="20" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J19" s="26"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="25"/>
+    </row>
+    <row r="20" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>13</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>12</v>
@@ -1303,14 +1546,18 @@
       </c>
       <c r="H20" s="13"/>
       <c r="I20" s="14"/>
-      <c r="J20" s="15"/>
-    </row>
-    <row r="21" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="26"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
         <v>14</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="6">
         <v>1</v>
@@ -1325,15 +1572,25 @@
         <v>120</v>
       </c>
       <c r="H21" s="13"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="15"/>
-    </row>
-    <row r="22" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="J21" s="34">
+        <v>3</v>
+      </c>
+      <c r="K21" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="L21" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
         <v>15</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="7" t="s">
@@ -1346,15 +1603,25 @@
         <v>90</v>
       </c>
       <c r="H22" s="13"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="15"/>
-    </row>
-    <row r="23" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="J22" s="34">
+        <v>3</v>
+      </c>
+      <c r="K22" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="L22" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
         <v>16</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="7" t="s">
@@ -1367,15 +1634,25 @@
         <v>90</v>
       </c>
       <c r="H23" s="13"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="15"/>
-    </row>
-    <row r="24" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="J23" s="34">
+        <v>3</v>
+      </c>
+      <c r="K23" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="L23" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
         <v>17</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="7" t="s">
@@ -1388,15 +1665,25 @@
         <v>60</v>
       </c>
       <c r="H24" s="13"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="15"/>
-    </row>
-    <row r="25" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="J24" s="34">
+        <v>3</v>
+      </c>
+      <c r="K24" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="L24" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
         <v>18</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="6">
         <v>8</v>
@@ -1405,50 +1692,60 @@
         <v>7</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G25" s="7">
         <v>240</v>
       </c>
       <c r="H25" s="13"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="15"/>
-    </row>
-    <row r="26" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="J25" s="34">
+        <v>3</v>
+      </c>
+      <c r="K25" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="L25" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="G26" s="20">
+      <c r="G26" s="17">
         <v>120</v>
       </c>
-      <c r="H26" s="20">
+      <c r="H26" s="17">
         <v>300</v>
       </c>
-      <c r="I26" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="J26" s="20"/>
+      <c r="I26" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J26" s="17"/>
     </row>
     <row r="27" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M28" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M29" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N29" s="12">
         <v>1875</v>
@@ -1456,11 +1753,11 @@
     </row>
     <row r="30" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="M30" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N30" s="12">
         <f>SUM(H4:H26)</f>
-        <v>860</v>
+        <v>2410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed attack sliding bug
</commit_message>
<xml_diff>
--- a/C61/Sprint 1/Planification.xlsx
+++ b/C61/Sprint 1/Planification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\ProjetFinalC61\C61\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7D20C7-7D89-4BB9-8DE8-D874A77D03E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE375BD8-E169-4A71-8A38-BE236B82B143}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11BE00C6-C346-4921-8AF1-FC1656D8A7FD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="72">
   <si>
     <t>Tâche</t>
   </si>
@@ -210,9 +210,6 @@
     <t>Long car a dû être refait, plusieurs bugs d'animation, beaucoup de lecture de doc</t>
   </si>
   <si>
-    <t xml:space="preserve">Pas de menu ou autre level pour le moment </t>
-  </si>
-  <si>
     <t>Finir un level complet et débuggé + main menu en priorité</t>
   </si>
   <si>
@@ -247,6 +244,12 @@
   </si>
   <si>
     <t xml:space="preserve">Plus long dû au changement de projet et gestion des colliders frame par frame </t>
+  </si>
+  <si>
+    <t>Autres options comme Settings et Load Game à venir, plus long car changement concept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas d'autre level pour le moment </t>
   </si>
 </sst>
 </file>
@@ -631,12 +634,6 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -649,6 +646,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -972,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2D228D-ED81-450E-98C6-898DFE30E920}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,25 +990,25 @@
     <col min="7" max="7" width="12.42578125" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="30"/>
+    <col min="11" max="11" width="11.42578125" style="28"/>
     <col min="12" max="12" width="100.140625" customWidth="1"/>
     <col min="13" max="13" width="15.28515625" customWidth="1"/>
     <col min="14" max="14" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" ht="63" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1033,7 +1036,7 @@
       <c r="J3" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="31" t="s">
+      <c r="K3" s="29" t="s">
         <v>53</v>
       </c>
       <c r="L3" s="24" t="s">
@@ -1064,7 +1067,7 @@
         <v>40</v>
       </c>
       <c r="J4" s="26"/>
-      <c r="K4" s="32" t="s">
+      <c r="K4" s="30" t="s">
         <v>54</v>
       </c>
       <c r="L4" s="25" t="s">
@@ -1097,8 +1100,8 @@
         <v>45</v>
       </c>
       <c r="J5" s="27"/>
-      <c r="K5" s="32" t="s">
-        <v>60</v>
+      <c r="K5" s="30" t="s">
+        <v>59</v>
       </c>
       <c r="L5" s="25"/>
     </row>
@@ -1128,7 +1131,7 @@
         <v>40</v>
       </c>
       <c r="J6" s="26"/>
-      <c r="K6" s="32" t="s">
+      <c r="K6" s="30" t="s">
         <v>54</v>
       </c>
       <c r="L6" s="25" t="s">
@@ -1161,8 +1164,8 @@
         <v>45</v>
       </c>
       <c r="J7" s="27"/>
-      <c r="K7" s="32" t="s">
-        <v>60</v>
+      <c r="K7" s="30" t="s">
+        <v>59</v>
       </c>
       <c r="L7" s="25" t="s">
         <v>52</v>
@@ -1192,8 +1195,8 @@
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="26"/>
-      <c r="K8" s="32" t="s">
-        <v>61</v>
+      <c r="K8" s="30" t="s">
+        <v>60</v>
       </c>
       <c r="L8" s="25" t="s">
         <v>51</v>
@@ -1223,8 +1226,8 @@
         <v>45</v>
       </c>
       <c r="J9" s="26"/>
-      <c r="K9" s="32" t="s">
-        <v>60</v>
+      <c r="K9" s="30" t="s">
+        <v>59</v>
       </c>
       <c r="L9" s="25"/>
     </row>
@@ -1250,11 +1253,11 @@
       </c>
       <c r="I10" s="14"/>
       <c r="J10" s="26"/>
-      <c r="K10" s="32" t="s">
-        <v>62</v>
+      <c r="K10" s="30" t="s">
+        <v>61</v>
       </c>
       <c r="L10" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1283,8 +1286,8 @@
         <v>40</v>
       </c>
       <c r="J11" s="26"/>
-      <c r="K11" s="32" t="s">
-        <v>60</v>
+      <c r="K11" s="30" t="s">
+        <v>59</v>
       </c>
       <c r="L11" s="25"/>
     </row>
@@ -1312,11 +1315,11 @@
       </c>
       <c r="I12" s="14"/>
       <c r="J12" s="26"/>
-      <c r="K12" s="32" t="s">
+      <c r="K12" s="30" t="s">
         <v>54</v>
       </c>
       <c r="L12" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1339,12 +1342,12 @@
         <v>120</v>
       </c>
       <c r="H13" s="13">
-        <v>300</v>
+        <v>340</v>
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="26"/>
-      <c r="K13" s="32" t="s">
-        <v>64</v>
+      <c r="K13" s="30" t="s">
+        <v>63</v>
       </c>
       <c r="L13" s="25" t="s">
         <v>57</v>
@@ -1374,8 +1377,8 @@
         <v>40</v>
       </c>
       <c r="J14" s="26"/>
-      <c r="K14" s="32" t="s">
-        <v>61</v>
+      <c r="K14" s="30" t="s">
+        <v>60</v>
       </c>
       <c r="L14" s="25"/>
     </row>
@@ -1402,14 +1405,14 @@
       <c r="I15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J15" s="34">
+      <c r="J15" s="32">
         <v>3</v>
       </c>
-      <c r="K15" s="32" t="s">
-        <v>65</v>
+      <c r="K15" s="30" t="s">
+        <v>64</v>
       </c>
       <c r="L15" s="25" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="M15" s="15"/>
     </row>
@@ -1437,8 +1440,8 @@
         <v>44</v>
       </c>
       <c r="J16" s="26"/>
-      <c r="K16" s="32" t="s">
-        <v>60</v>
+      <c r="K16" s="30" t="s">
+        <v>59</v>
       </c>
       <c r="L16" s="25"/>
     </row>
@@ -1466,8 +1469,8 @@
         <v>44</v>
       </c>
       <c r="J17" s="26"/>
-      <c r="K17" s="32" t="s">
-        <v>60</v>
+      <c r="K17" s="30" t="s">
+        <v>59</v>
       </c>
       <c r="L17" s="25"/>
     </row>
@@ -1493,11 +1496,11 @@
       </c>
       <c r="I18" s="14"/>
       <c r="J18" s="26"/>
-      <c r="K18" s="32" t="s">
-        <v>66</v>
+      <c r="K18" s="30" t="s">
+        <v>65</v>
       </c>
       <c r="L18" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1519,18 +1522,24 @@
       <c r="G19" s="7">
         <v>60</v>
       </c>
-      <c r="H19" s="13"/>
+      <c r="H19" s="13">
+        <v>150</v>
+      </c>
       <c r="I19" s="14"/>
       <c r="J19" s="26"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="25"/>
+      <c r="K19" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="L19" s="25" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="20" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>13</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>12</v>
@@ -1547,9 +1556,9 @@
       <c r="H20" s="13"/>
       <c r="I20" s="14"/>
       <c r="J20" s="26"/>
-      <c r="K20" s="32"/>
+      <c r="K20" s="30"/>
       <c r="L20" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1575,14 +1584,14 @@
       <c r="I21" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="34">
+      <c r="J21" s="32">
         <v>3</v>
       </c>
-      <c r="K21" s="32" t="s">
-        <v>60</v>
+      <c r="K21" s="30" t="s">
+        <v>59</v>
       </c>
       <c r="L21" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1606,14 +1615,14 @@
       <c r="I22" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J22" s="34">
+      <c r="J22" s="32">
         <v>3</v>
       </c>
-      <c r="K22" s="32" t="s">
-        <v>60</v>
+      <c r="K22" s="30" t="s">
+        <v>59</v>
       </c>
       <c r="L22" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1637,14 +1646,14 @@
       <c r="I23" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J23" s="34">
+      <c r="J23" s="32">
         <v>3</v>
       </c>
-      <c r="K23" s="32" t="s">
-        <v>60</v>
+      <c r="K23" s="30" t="s">
+        <v>59</v>
       </c>
       <c r="L23" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1668,14 +1677,14 @@
       <c r="I24" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J24" s="34">
+      <c r="J24" s="32">
         <v>3</v>
       </c>
-      <c r="K24" s="32" t="s">
-        <v>60</v>
+      <c r="K24" s="30" t="s">
+        <v>59</v>
       </c>
       <c r="L24" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1701,14 +1710,14 @@
       <c r="I25" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J25" s="34">
+      <c r="J25" s="32">
         <v>3</v>
       </c>
-      <c r="K25" s="33" t="s">
-        <v>60</v>
+      <c r="K25" s="31" t="s">
+        <v>59</v>
       </c>
       <c r="L25" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1757,7 +1766,7 @@
       </c>
       <c r="N30" s="12">
         <f>SUM(H4:H26)</f>
-        <v>2410</v>
+        <v>2600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>